<commit_message>
Training on Camping Data
Train , Test and Validation on Camping Dataset
</commit_message>
<xml_diff>
--- a/Camping_OM_Resources/Dataset/Camping1_Samples_on_current_model.xlsx
+++ b/Camping_OM_Resources/Dataset/Camping1_Samples_on_current_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rashedhasan/Desktop/UNL/Research/Object relational mapping/Step 5 - Abstraction/OM-Solution_Mapping/OM-ML_Research/Camping_OM_Resources/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1891AA28-2C6C-6A4A-BBB3-1B0D5CD1B37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5678C6A-4E62-3940-99CA-AB806AAD065C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{7828C3CB-928D-DD4C-ABD5-580F5D69FBC1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="100">
   <si>
     <t>OM_Regular</t>
   </si>
@@ -718,13 +718,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3EFDD74-2AE0-AB4A-9475-FAE3E9FDAC91}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="116.1640625" customWidth="1"/>
+    <col min="1" max="1" width="118.33203125" customWidth="1"/>
     <col min="2" max="2" width="94.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -846,7 +846,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
@@ -854,7 +854,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B17" t="s">
@@ -862,12 +862,15 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B19" t="s">
@@ -875,7 +878,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
@@ -883,7 +886,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B21" t="s">
@@ -891,7 +894,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
@@ -899,7 +902,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
@@ -907,7 +910,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B24" t="s">
@@ -915,7 +918,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B25" t="s">
@@ -923,7 +926,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B26" t="s">
@@ -931,7 +934,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B27" t="s">
@@ -939,7 +942,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B28" t="s">
@@ -947,7 +950,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B29" t="s">
@@ -955,7 +958,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B30" t="s">
@@ -963,7 +966,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B31" t="s">
@@ -971,7 +974,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B32" t="s">
@@ -979,8 +982,11 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1037,7 +1043,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B42" t="s">
@@ -1045,7 +1051,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B43" t="s">
@@ -1053,7 +1059,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B44" t="s">
@@ -1061,7 +1067,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B45" t="s">
@@ -1069,7 +1075,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B46" t="s">
@@ -1077,7 +1083,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B47" t="s">
@@ -1085,7 +1091,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B48" t="s">
@@ -1093,7 +1099,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B49" t="s">
@@ -1101,12 +1107,15 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="B50" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B51" t="s">
@@ -1114,7 +1123,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B52" t="s">
@@ -1122,7 +1131,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B53" t="s">
@@ -1130,7 +1139,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B54" t="s">
@@ -1138,7 +1147,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B55" t="s">
@@ -1146,7 +1155,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B56" t="s">
@@ -1154,7 +1163,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B57" t="s">
@@ -1162,7 +1171,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B58" t="s">
@@ -1170,7 +1179,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B59" t="s">
@@ -1178,7 +1187,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B60" t="s">
@@ -1186,7 +1195,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B61" t="s">
@@ -1194,7 +1203,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B62" t="s">
@@ -1202,7 +1211,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B63" t="s">
@@ -1210,16 +1219,19 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="A64" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B64" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>94</v>
+      </c>
+      <c r="B65" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>